<commit_message>
Added helpers for week 3 activities
</commit_message>
<xml_diff>
--- a/src/data/paralympics.xlsx
+++ b/src/data/paralympics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahsanders/PycharmProjects/comp0034-tutorials-2025/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1169A3EE-F7F3-D64C-9F2E-F7E454F7A6D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53BE26F-EE25-2A46-87C8-8F3314F61763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8840" yWindow="-22620" windowWidth="28040" windowHeight="17200" xr2:uid="{CBF15B4E-2805-CD44-9DA6-567684115F1A}"/>
+    <workbookView xWindow="5880" yWindow="-21000" windowWidth="28040" windowHeight="17200" xr2:uid="{CBF15B4E-2805-CD44-9DA6-567684115F1A}"/>
   </bookViews>
   <sheets>
     <sheet name="games" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4383" uniqueCount="840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4422" uniqueCount="846">
   <si>
     <t>type</t>
   </si>
@@ -2560,14 +2560,32 @@
     <t>A separate event for wheelchair athletes.</t>
   </si>
   <si>
-    <t>NOT</t>
+    <t>country_code</t>
+  </si>
+  <si>
+    <t>country_name</t>
+  </si>
+  <si>
+    <t>Korea</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2706,6 +2724,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -3050,13 +3074,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3432,20 +3457,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A5B346-9586-614E-9210-4DD6279EFFF5}">
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="Q1" sqref="Q1:R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3453,46 +3480,55 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>839</v>
       </c>
       <c r="D1" t="s">
+        <v>840</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q1" t="s">
+        <v>844</v>
+      </c>
+      <c r="R1" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -3503,37 +3539,46 @@
         <v>185</v>
       </c>
       <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>22177</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>22184</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>23</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>113</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>8</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>209</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>18</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q2" s="4">
+        <v>41.893099999999997</v>
+      </c>
+      <c r="R2" s="4">
+        <v>12.482799999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -3544,43 +3589,52 @@
         <v>186</v>
       </c>
       <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>23689</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>23693</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>17</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>21</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>143</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>9</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>195</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>71</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>266</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>21</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q3" s="4">
+        <v>35.689700000000002</v>
+      </c>
+      <c r="R3" s="4">
+        <v>139.69220000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -3591,43 +3645,52 @@
         <v>206</v>
       </c>
       <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>25147</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>25156</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>17</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>29</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>188</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>10</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>578</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>196</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>774</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>24</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q4" s="4">
+        <v>32.08</v>
+      </c>
+      <c r="R4" s="4">
+        <v>34.78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -3638,43 +3701,52 @@
         <v>172</v>
       </c>
       <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>26513</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>26522</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>17</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>43</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>188</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>10</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>654</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>268</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>922</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>27</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q5" s="4">
+        <v>49.412199999999999</v>
+      </c>
+      <c r="R5" s="4">
+        <v>8.7100000000000009</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -3685,43 +3757,52 @@
         <v>176</v>
       </c>
       <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>27976</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>27984</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>30</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>40</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>448</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>13</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>1000</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>271</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>1271</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>31</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q6" s="4">
+        <v>43.653199999999998</v>
+      </c>
+      <c r="R6" s="4">
+        <v>-79.383200000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -3732,43 +3813,52 @@
         <v>179</v>
       </c>
       <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>29394</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>29403</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>34</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>43</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>590</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>13</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>1225</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>428</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>1653</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>35</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q7" s="4">
+        <v>51.9833</v>
+      </c>
+      <c r="R7" s="4">
+        <v>5.9166999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3779,43 +3869,52 @@
         <v>173</v>
       </c>
       <c r="D8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" t="s">
         <v>836</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>30885</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>30895</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>34</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>41</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>975</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>18</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>1569</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>536</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>1100</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>838</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q8" s="4">
+        <v>51.786099999999998</v>
+      </c>
+      <c r="R8" s="4">
+        <v>-0.79139999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -3825,44 +3924,53 @@
       <c r="C9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E9" t="s">
         <v>837</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>30849</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <v>30863</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>34</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>54</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>975</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>18</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>1569</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>536</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>1800</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>36</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q9" s="4">
+        <v>40.712800000000001</v>
+      </c>
+      <c r="R9" s="4">
+        <v>-74.006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -3873,43 +3981,52 @@
         <v>182</v>
       </c>
       <c r="D10" t="s">
+        <v>841</v>
+      </c>
+      <c r="E10" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>32432</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <v>32441</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>34</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>60</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>733</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>18</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>2370</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>671</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>3041</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>38</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q10" s="4">
+        <v>37.56</v>
+      </c>
+      <c r="R10" s="4">
+        <v>126.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -3920,43 +4037,52 @@
         <v>175</v>
       </c>
       <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>33852</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G11" s="1">
         <v>33863</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>34</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>83</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>489</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>16</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>2300</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>699</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>2999</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>41</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q11" s="4">
+        <v>41.3825</v>
+      </c>
+      <c r="R11" s="4">
+        <v>2.1768999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -3966,44 +4092,53 @@
       <c r="C12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <v>35293</v>
       </c>
-      <c r="F12" s="1">
+      <c r="G12" s="1">
         <v>35302</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>44</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>104</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>519</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>19</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>2462</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>790</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>3252</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>45</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q12" s="4">
+        <v>33.749000000000002</v>
+      </c>
+      <c r="R12" s="4">
+        <v>-84.388000000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -4014,43 +4149,52 @@
         <v>177</v>
       </c>
       <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
         <v>36822</v>
       </c>
-      <c r="F13" s="1">
+      <c r="G13" s="1">
         <v>36830</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>44</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>123</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>550</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>19</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>2883</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>988</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>3871</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>48</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q13" s="4">
+        <v>-33.8688</v>
+      </c>
+      <c r="R13" s="4">
+        <v>151.20930000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -4061,43 +4205,52 @@
         <v>221</v>
       </c>
       <c r="D14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
         <v>38253</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14" s="1">
         <v>38264</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>34</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>135</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>519</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>19</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>2600</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>1149</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>3749</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>51</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q14" s="4">
+        <v>37.983800000000002</v>
+      </c>
+      <c r="R14" s="4">
+        <v>23.727499999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -4108,43 +4261,52 @@
         <v>183</v>
       </c>
       <c r="D15" t="s">
+        <v>842</v>
+      </c>
+      <c r="E15" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
         <v>39697</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15" s="1">
         <v>39708</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>34</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>146</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>472</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>20</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>2585</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>1366</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>3951</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>53</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q15" s="4">
+        <v>39.904200000000003</v>
+      </c>
+      <c r="R15" s="4">
+        <v>116.4074</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -4155,43 +4317,52 @@
         <v>173</v>
       </c>
       <c r="D16" t="s">
+        <v>134</v>
+      </c>
+      <c r="E16" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <v>41150</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="1">
         <v>41161</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>44</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>164</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>530</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>20</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>2741</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>1502</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>4243</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>55</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q16" s="4">
+        <v>51.507199999999997</v>
+      </c>
+      <c r="R16" s="4">
+        <v>0.12759999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -4202,43 +4373,52 @@
         <v>203</v>
       </c>
       <c r="D17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <v>42620</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G17" s="1">
         <v>42631</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>44</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>160</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>528</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>22</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>2657</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>1670</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>4327</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>58</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q17" s="4">
+        <v>-22.9068</v>
+      </c>
+      <c r="R17" s="4">
+        <v>-43.172899999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -4249,43 +4429,52 @@
         <v>186</v>
       </c>
       <c r="D18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <v>44432</v>
       </c>
-      <c r="F18" s="1">
+      <c r="G18" s="1">
         <v>44444</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>44</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>162</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>539</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>22</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>2547</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>1846</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>4393</v>
       </c>
-      <c r="N18" t="s">
+      <c r="O18" t="s">
         <v>59</v>
       </c>
-      <c r="O18" t="s">
+      <c r="P18" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q18" s="4">
+        <v>35.689700000000002</v>
+      </c>
+      <c r="R18" s="4">
+        <v>139.69220000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -4296,43 +4485,52 @@
         <v>174</v>
       </c>
       <c r="D19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <v>45532</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G19" s="1">
         <v>45543</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>44</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>169</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>549</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>22</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>2551</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>2016</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>4567</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>368</v>
       </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q19" s="4">
+        <v>48.864716000000001</v>
+      </c>
+      <c r="R19" s="4">
+        <v>2.3490139999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -4342,26 +4540,35 @@
       <c r="C20" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E20" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <v>46980</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G20" s="1">
         <v>46992</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>44</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>22</v>
       </c>
-      <c r="O20" t="s">
+      <c r="P20" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q20" s="4">
+        <v>34.052235000000003</v>
+      </c>
+      <c r="R20" s="4">
+        <v>-118.243683</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -4372,19 +4579,28 @@
         <v>177</v>
       </c>
       <c r="D21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" t="s">
         <v>371</v>
       </c>
-      <c r="E21" s="1">
+      <c r="F21" s="1">
         <v>48450</v>
       </c>
-      <c r="F21" s="1">
+      <c r="G21" s="1">
         <v>48462</v>
       </c>
-      <c r="O21" t="s">
+      <c r="P21" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q21" s="4">
+        <v>-27.470124999999999</v>
+      </c>
+      <c r="R21" s="4">
+        <v>153.021072</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>369</v>
       </c>
@@ -4395,43 +4611,52 @@
         <v>188</v>
       </c>
       <c r="D22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" t="s">
         <v>65</v>
       </c>
-      <c r="E22" s="1">
+      <c r="F22" s="1">
         <v>27811</v>
       </c>
-      <c r="F22" s="1">
+      <c r="G22" s="1">
         <v>27818</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>17</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>16</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>53</v>
       </c>
-      <c r="J22">
-        <v>2</v>
-      </c>
       <c r="K22">
+        <v>2</v>
+      </c>
+      <c r="L22">
         <v>161</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <v>37</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <v>198</v>
       </c>
-      <c r="N22" t="s">
+      <c r="O22" t="s">
         <v>66</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P22" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q22" s="4">
+        <v>63.29</v>
+      </c>
+      <c r="R22" s="4">
+        <v>18.7166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -4442,43 +4667,52 @@
         <v>180</v>
       </c>
       <c r="D23" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" t="s">
         <v>68</v>
       </c>
-      <c r="E23" s="1">
+      <c r="F23" s="1">
         <v>29253</v>
       </c>
-      <c r="F23" s="1">
+      <c r="G23" s="1">
         <v>29259</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>30</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>18</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>64</v>
       </c>
-      <c r="J23">
-        <v>2</v>
-      </c>
       <c r="K23">
+        <v>2</v>
+      </c>
+      <c r="L23">
         <v>229</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <v>70</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <v>299</v>
       </c>
-      <c r="N23" t="s">
+      <c r="O23" t="s">
         <v>69</v>
       </c>
-      <c r="O23" t="s">
+      <c r="P23" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q23" s="4">
+        <v>60.533700000000003</v>
+      </c>
+      <c r="R23" s="4">
+        <v>8.2088000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -4489,43 +4723,52 @@
         <v>192</v>
       </c>
       <c r="D24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="1">
+      <c r="F24" s="1">
         <v>30696</v>
       </c>
-      <c r="F24" s="1">
+      <c r="G24" s="1">
         <v>30702</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>34</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>21</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>107</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>3</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>325</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <v>94</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>419</v>
       </c>
-      <c r="N24" t="s">
+      <c r="O24" t="s">
         <v>72</v>
       </c>
-      <c r="O24" t="s">
+      <c r="P24" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q24" s="4">
+        <v>47.269199999999998</v>
+      </c>
+      <c r="R24" s="4">
+        <v>11.4041</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -4536,43 +4779,52 @@
         <v>192</v>
       </c>
       <c r="D25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" t="s">
         <v>71</v>
       </c>
-      <c r="E25" s="1">
+      <c r="F25" s="1">
         <v>32160</v>
       </c>
-      <c r="F25" s="1">
+      <c r="G25" s="1">
         <v>32167</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>34</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>22</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>97</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>4</v>
       </c>
-      <c r="K25">
+      <c r="L25">
         <v>300</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <v>77</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <v>377</v>
       </c>
-      <c r="N25" t="s">
+      <c r="O25" t="s">
         <v>73</v>
       </c>
-      <c r="O25" t="s">
+      <c r="P25" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q25" s="4">
+        <v>47.269199999999998</v>
+      </c>
+      <c r="R25" s="4">
+        <v>11.4041</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>63</v>
       </c>
@@ -4583,43 +4835,52 @@
         <v>174</v>
       </c>
       <c r="D26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" t="s">
         <v>74</v>
       </c>
-      <c r="E26" s="1">
+      <c r="F26" s="1">
         <v>33688</v>
       </c>
-      <c r="F26" s="1">
+      <c r="G26" s="1">
         <v>33696</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>34</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>24</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>79</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>3</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <v>288</v>
       </c>
-      <c r="L26">
+      <c r="M26">
         <v>77</v>
       </c>
-      <c r="M26">
+      <c r="N26">
         <v>365</v>
       </c>
-      <c r="N26" t="s">
+      <c r="O26" t="s">
         <v>75</v>
       </c>
-      <c r="O26" t="s">
+      <c r="P26" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q26" s="4">
+        <v>45.468299999999999</v>
+      </c>
+      <c r="R26" s="4">
+        <v>6.9055999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -4627,46 +4888,55 @@
         <v>1994</v>
       </c>
       <c r="C27" t="s">
-        <v>839</v>
+        <v>180</v>
       </c>
       <c r="D27" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" t="s">
         <v>76</v>
       </c>
-      <c r="E27" s="1">
+      <c r="F27" s="1">
         <v>34403</v>
       </c>
-      <c r="F27" s="1">
+      <c r="G27" s="1">
         <v>34412</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>34</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>31</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>133</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>5</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <v>39</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <v>90</v>
       </c>
-      <c r="M27">
+      <c r="N27">
         <v>129</v>
       </c>
-      <c r="N27" t="s">
+      <c r="O27" t="s">
         <v>77</v>
       </c>
-      <c r="O27" t="s">
+      <c r="P27" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q27" s="4">
+        <v>61.115299999999998</v>
+      </c>
+      <c r="R27" s="4">
+        <v>10.466200000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -4677,43 +4947,52 @@
         <v>186</v>
       </c>
       <c r="D28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" t="s">
         <v>78</v>
       </c>
-      <c r="E28" s="1">
+      <c r="F28" s="1">
         <v>35861</v>
       </c>
-      <c r="F28" s="1">
+      <c r="G28" s="1">
         <v>35870</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>34</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>31</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>122</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>5</v>
       </c>
-      <c r="K28">
+      <c r="L28">
         <v>440</v>
       </c>
-      <c r="L28">
+      <c r="M28">
         <v>122</v>
       </c>
-      <c r="M28">
+      <c r="N28">
         <v>562</v>
       </c>
-      <c r="N28" t="s">
+      <c r="O28" t="s">
         <v>79</v>
       </c>
-      <c r="O28" t="s">
+      <c r="P28" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q28" s="4">
+        <v>36.648499999999999</v>
+      </c>
+      <c r="R28" s="4">
+        <v>138.19499999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -4723,44 +5002,53 @@
       <c r="C29" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E29" t="s">
         <v>80</v>
       </c>
-      <c r="E29" s="1">
+      <c r="F29" s="1">
         <v>37324</v>
       </c>
-      <c r="F29" s="1">
+      <c r="G29" s="1">
         <v>37333</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>34</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>36</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>92</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>4</v>
       </c>
-      <c r="K29">
+      <c r="L29">
         <v>328</v>
       </c>
-      <c r="L29">
+      <c r="M29">
         <v>87</v>
       </c>
-      <c r="M29">
+      <c r="N29">
         <v>415</v>
       </c>
-      <c r="N29" t="s">
+      <c r="O29" t="s">
         <v>81</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q29" s="4">
+        <v>40.760800000000003</v>
+      </c>
+      <c r="R29" s="4">
+        <v>-111.89100000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -4771,43 +5059,52 @@
         <v>185</v>
       </c>
       <c r="D30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" t="s">
         <v>82</v>
       </c>
-      <c r="E30" s="1">
+      <c r="F30" s="1">
         <v>38788</v>
       </c>
-      <c r="F30" s="1">
+      <c r="G30" s="1">
         <v>38797</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>34</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>38</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>58</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>5</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <v>375</v>
       </c>
-      <c r="L30">
+      <c r="M30">
         <v>99</v>
       </c>
-      <c r="M30">
+      <c r="N30">
         <v>474</v>
       </c>
-      <c r="N30" t="s">
+      <c r="O30" t="s">
         <v>83</v>
       </c>
-      <c r="O30" t="s">
+      <c r="P30" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q30" s="4">
+        <v>45.070300000000003</v>
+      </c>
+      <c r="R30" s="4">
+        <v>7.6868999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -4818,43 +5115,52 @@
         <v>176</v>
       </c>
       <c r="D31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" t="s">
         <v>84</v>
       </c>
-      <c r="E31" s="1">
+      <c r="F31" s="1">
         <v>40249</v>
       </c>
-      <c r="F31" s="1">
+      <c r="G31" s="1">
         <v>40258</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>34</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>44</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>64</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>5</v>
       </c>
-      <c r="K31">
+      <c r="L31">
         <v>381</v>
       </c>
-      <c r="L31">
+      <c r="M31">
         <v>121</v>
       </c>
-      <c r="M31">
+      <c r="N31">
         <v>502</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>85</v>
       </c>
-      <c r="O31" t="s">
+      <c r="P31" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q31" s="4">
+        <v>49.282699999999998</v>
+      </c>
+      <c r="R31" s="4">
+        <v>-123.1207</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -4865,43 +5171,52 @@
         <v>237</v>
       </c>
       <c r="D32" t="s">
+        <v>843</v>
+      </c>
+      <c r="E32" t="s">
         <v>86</v>
       </c>
-      <c r="E32" s="1">
+      <c r="F32" s="1">
         <v>41705</v>
       </c>
-      <c r="F32" s="1">
+      <c r="G32" s="1">
         <v>41714</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>34</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <v>45</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>72</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <v>6</v>
       </c>
-      <c r="K32">
+      <c r="L32">
         <v>411</v>
       </c>
-      <c r="L32">
+      <c r="M32">
         <v>129</v>
       </c>
-      <c r="M32">
+      <c r="N32">
         <v>540</v>
       </c>
-      <c r="N32" t="s">
+      <c r="O32" t="s">
         <v>87</v>
       </c>
-      <c r="O32" t="s">
+      <c r="P32" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q32" s="4">
+        <v>43.602800000000002</v>
+      </c>
+      <c r="R32" s="4">
+        <v>39.734200000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -4912,43 +5227,52 @@
         <v>182</v>
       </c>
       <c r="D33" t="s">
+        <v>841</v>
+      </c>
+      <c r="E33" t="s">
         <v>88</v>
       </c>
-      <c r="E33" s="1">
+      <c r="F33" s="1">
         <v>43168</v>
       </c>
-      <c r="F33" s="1">
+      <c r="G33" s="1">
         <v>43177</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>89</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>49</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>80</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>6</v>
       </c>
-      <c r="K33">
+      <c r="L33">
         <v>430</v>
       </c>
-      <c r="L33">
+      <c r="M33">
         <v>133</v>
       </c>
-      <c r="M33">
+      <c r="N33">
         <v>563</v>
       </c>
-      <c r="N33" t="s">
+      <c r="O33" t="s">
         <v>90</v>
       </c>
-      <c r="O33" t="s">
+      <c r="P33" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q33" s="4">
+        <v>37.3705</v>
+      </c>
+      <c r="R33" s="4">
+        <v>128.38999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -4959,43 +5283,52 @@
         <v>183</v>
       </c>
       <c r="D34" t="s">
+        <v>842</v>
+      </c>
+      <c r="E34" t="s">
         <v>52</v>
       </c>
-      <c r="E34" s="1">
+      <c r="F34" s="1">
         <v>44624</v>
       </c>
-      <c r="F34" s="1">
+      <c r="G34" s="1">
         <v>44633</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>89</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>46</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>78</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <v>6</v>
       </c>
-      <c r="K34">
+      <c r="L34">
         <v>422</v>
       </c>
-      <c r="L34">
+      <c r="M34">
         <v>136</v>
       </c>
-      <c r="M34">
+      <c r="N34">
         <v>558</v>
       </c>
-      <c r="N34" t="s">
+      <c r="O34" t="s">
         <v>91</v>
       </c>
-      <c r="O34" t="s">
+      <c r="P34" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q34" s="4">
+        <v>39.904200000000003</v>
+      </c>
+      <c r="R34" s="4">
+        <v>116.4074</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -5006,28 +5339,37 @@
         <v>185</v>
       </c>
       <c r="D35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" t="s">
         <v>92</v>
       </c>
-      <c r="E35" s="1">
+      <c r="F35" s="1">
         <v>46087</v>
       </c>
-      <c r="F35" s="1">
+      <c r="G35" s="1">
         <v>46096</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>89</v>
       </c>
-      <c r="I35">
+      <c r="J35">
         <v>79</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <v>6</v>
       </c>
-      <c r="O35" t="s">
+      <c r="P35" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q35" s="4">
+        <v>45.464663999999999</v>
+      </c>
+      <c r="R35" s="4">
+        <v>9.1885399999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>63</v>
       </c>
@@ -5038,19 +5380,28 @@
         <v>174</v>
       </c>
       <c r="D36" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" t="s">
         <v>370</v>
       </c>
-      <c r="E36" s="1">
+      <c r="F36" s="1">
         <v>47543</v>
       </c>
-      <c r="F36" s="1">
+      <c r="G36" s="1">
         <v>47552</v>
       </c>
-      <c r="O36" t="s">
+      <c r="P36" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="Q36" s="4">
+        <v>45.833599999999997</v>
+      </c>
+      <c r="R36" s="4">
+        <v>6.8650000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>63</v>
       </c>
@@ -5060,17 +5411,26 @@
       <c r="C37" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E37" t="s">
         <v>80</v>
       </c>
-      <c r="E37" s="1">
+      <c r="F37" s="1">
         <v>49013</v>
       </c>
-      <c r="F37" s="1">
+      <c r="G37" s="1">
         <v>49022</v>
       </c>
-      <c r="O37" t="s">
+      <c r="P37" t="s">
         <v>374</v>
+      </c>
+      <c r="Q37" s="4">
+        <v>40.760800000000003</v>
+      </c>
+      <c r="R37" s="4">
+        <v>-111.89100000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>